<commit_message>
ReLU with small dataset.  Seems to be working.
</commit_message>
<xml_diff>
--- a/Applications/MNIST/Step03_SetupNeuralNetwork/Step03_IDs.xlsx
+++ b/Applications/MNIST/Step03_SetupNeuralNetwork/Step03_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MatlabAIML\Applications\MNIST\Step03_SetupNeuralNetwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2771097-553D-4C82-B2D3-284B5FAFA327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BEE47E-8E29-4B70-BEC9-9D30898C4DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="19905" yWindow="-14370" windowWidth="21600" windowHeight="15435" xr2:uid="{62938247-60B1-4176-96BA-8E8C4D4BE688}"/>
+    <workbookView xWindow="-8325" yWindow="-15870" windowWidth="25440" windowHeight="15990" xr2:uid="{62938247-60B1-4176-96BA-8E8C4D4BE688}"/>
   </bookViews>
   <sheets>
     <sheet name="Step03A" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Comment</t>
   </si>
@@ -56,9 +56,6 @@
     <t>[28*28 50 10]</t>
   </si>
   <si>
-    <t>all sigmoid</t>
-  </si>
-  <si>
     <t>NeuralNetworkScenario1.mat</t>
   </si>
   <si>
@@ -84,6 +81,21 @@
   </si>
   <si>
     <t>NeuralNetworkScenario4.mat</t>
+  </si>
+  <si>
+    <t>[N/A; ReLU; Sigmoid]</t>
+  </si>
+  <si>
+    <t>[N/A; Sigmoid; Sigmoid]</t>
+  </si>
+  <si>
+    <t>NeuralNetworkScenario5.mat</t>
+  </si>
+  <si>
+    <t>Partially trained network</t>
+  </si>
+  <si>
+    <t>only about a 50% accuracy</t>
   </si>
 </sst>
 </file>
@@ -456,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2242A2-D373-44A6-9DF2-E2416E056A77}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,55 +515,78 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>